<commit_message>
update webapp removing dependency to Clarity
</commit_message>
<xml_diff>
--- a/data/GEP00001/GEP00001.xlsx
+++ b/data/GEP00001/GEP00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="37620" yWindow="0" windowWidth="29100" windowHeight="19640" tabRatio="585"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="585" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4324" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4322" uniqueCount="468">
   <si>
     <t>geid</t>
   </si>
@@ -1804,7 +1804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1894,77 +1894,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
-    <col min="7" max="1024" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="1023" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>465</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>466</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
       <c r="E2">
-        <v>17</v>
+        <v>40465342</v>
       </c>
       <c r="F2">
-        <v>40465342</v>
-      </c>
-      <c r="G2">
         <v>40540586</v>
       </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
       <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2540,7 +2534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>